<commit_message>
Nộp sau phản biện
- Thêm được quiz cho video bài giảng
- Thêm được certificate
</commit_message>
<xml_diff>
--- a/doneWeb/QuestionpoolHtmlCss.xlsx
+++ b/doneWeb/QuestionpoolHtmlCss.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\02-07-2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChauHuynhPhuocToan\WebBackup - Copy - Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26970" windowHeight="10950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26976" windowHeight="10956"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>Quiz</t>
   </si>
@@ -150,12 +150,15 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -491,15 +494,15 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -554,7 +557,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I2" s="1">
         <v>10</v>
@@ -564,7 +567,7 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -580,9 +583,11 @@
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="H3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3" s="1">
         <v>10</v>
@@ -592,7 +597,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -622,7 +627,7 @@
       </c>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -642,7 +647,7 @@
         <v>29</v>
       </c>
       <c r="H5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I5" s="1">
         <v>20</v>
@@ -652,7 +657,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -682,7 +687,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -705,14 +710,14 @@
         <v>4</v>
       </c>
       <c r="I7" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J7" s="1">
         <v>60</v>
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -735,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="I8" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J8" s="1">
         <v>60</v>

</xml_diff>